<commit_message>
PASS BASELINE!!! both, noHazard & hasHazard!!!
</commit_message>
<xml_diff>
--- a/ref/Instruction2Binary2.xlsx
+++ b/ref/Instruction2Binary2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="Inst2BinCode" sheetId="1" r:id="rId1"/>
@@ -675,10 +675,30 @@
     <t>1</t>
   </si>
   <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sa hardwire into ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -687,10 +707,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rs &lt;- PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUFunction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -699,23 +751,153 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sa hardwire into ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
+    <t>NO ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100010</t>
+  </si>
+  <si>
+    <t>100100</t>
+  </si>
+  <si>
+    <t>100101</t>
+  </si>
+  <si>
+    <t>100110</t>
+  </si>
+  <si>
+    <t>100111</t>
+  </si>
+  <si>
+    <t>000011</t>
+  </si>
+  <si>
+    <t>000010</t>
+  </si>
+  <si>
+    <t>101010</t>
+  </si>
+  <si>
+    <t>001000</t>
+  </si>
+  <si>
+    <t>001001</t>
+  </si>
+  <si>
+    <t>OR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equal (reduced by sub&amp;zero)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SLT </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BEQ (SUB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -723,189 +905,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rs &lt;- PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALUFunction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SUB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100010</t>
-  </si>
-  <si>
-    <t>100100</t>
-  </si>
-  <si>
-    <t>100101</t>
-  </si>
-  <si>
-    <t>100110</t>
-  </si>
-  <si>
-    <t>100111</t>
-  </si>
-  <si>
-    <t>000011</t>
-  </si>
-  <si>
-    <t>000010</t>
-  </si>
-  <si>
-    <t>101010</t>
-  </si>
-  <si>
-    <t>001000</t>
-  </si>
-  <si>
-    <t>001001</t>
-  </si>
-  <si>
-    <t>OR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XOR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Equal (reduced by sub&amp;zero)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">SLT </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BEQ (SUB)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -962,7 +962,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -993,6 +993,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1008,7 +1014,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1039,12 +1045,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1052,9 +1052,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1068,6 +1065,27 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1351,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1449,11 +1467,11 @@
       <c r="E3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1541,11 +1559,11 @@
       <c r="E6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="3" t="s">
         <v>83</v>
       </c>
@@ -1601,11 +1619,11 @@
       <c r="E8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="3" t="s">
         <v>152</v>
       </c>
@@ -1661,11 +1679,11 @@
       <c r="E10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="3" t="s">
         <v>153</v>
       </c>
@@ -1706,105 +1724,105 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="K12" s="13" t="s">
-        <v>175</v>
+      <c r="K12" s="11" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="12"/>
+      <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="K14" s="12"/>
+      <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
@@ -1854,11 +1872,11 @@
       <c r="E16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
       <c r="I16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1874,7 +1892,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>37</v>
@@ -1882,11 +1900,11 @@
       <c r="E17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="2" t="s">
         <v>159</v>
       </c>
@@ -1904,13 +1922,13 @@
       <c r="C18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
       <c r="I18" s="2" t="s">
         <v>160</v>
       </c>
@@ -1928,18 +1946,18 @@
       <c r="C19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1955,16 +1973,16 @@
       <c r="D20" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
       <c r="H20" s="2" t="s">
         <v>138</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>139</v>
@@ -1996,7 +2014,7 @@
         <v>140</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>141</v>
@@ -2018,11 +2036,11 @@
       <c r="E22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
       <c r="I22" s="2" t="s">
         <v>157</v>
       </c>
@@ -2046,11 +2064,11 @@
       <c r="E23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="2" t="s">
         <v>157</v>
       </c>
@@ -2065,17 +2083,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2088,7 +2106,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2122,7 +2140,7 @@
         <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>50</v>
@@ -2146,12 +2164,12 @@
         <v>54</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q1" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="11"/>
+      <c r="R1" s="18"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -2200,44 +2218,45 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
+    <row r="3" spans="1:18" s="19" customFormat="1">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="20">
         <v>0</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="K3" s="8" t="s">
+      <c r="M3" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="20" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2335,44 +2354,45 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
-      <c r="A6" t="s">
+    <row r="6" spans="1:18" s="19" customFormat="1">
+      <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="20">
         <v>0</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" s="9" t="s">
+      <c r="H6" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="20" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2423,44 +2443,45 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
-      <c r="A8" t="s">
+    <row r="8" spans="1:18" s="19" customFormat="1">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="20"/>
+      <c r="E8" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="20">
         <v>0</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M8" s="9" t="s">
+      <c r="H8" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="20" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2511,44 +2532,45 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
-      <c r="A10" t="s">
+    <row r="10" spans="1:18" s="19" customFormat="1">
+      <c r="A10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="20">
         <v>0</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M10" s="9" t="s">
+      <c r="H10" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="20" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2616,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>164</v>
@@ -2657,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>169</v>
+        <v>227</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>165</v>
@@ -2698,10 +2720,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>170</v>
+        <v>228</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>63</v>
@@ -2739,7 +2761,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>164</v>
@@ -2763,44 +2785,45 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
-      <c r="A16" t="s">
+    <row r="16" spans="1:18" s="19" customFormat="1">
+      <c r="A16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="D16" s="20"/>
+      <c r="E16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="20">
         <v>0</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M16" s="9" t="s">
+      <c r="G16" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="20" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2812,7 +2835,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>65</v>
@@ -2945,36 +2968,36 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
-      <c r="A20" t="s">
+    <row r="20" spans="1:18" s="22" customFormat="1">
+      <c r="A20" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="E20" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20" s="23">
         <v>1</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>165</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>164</v>
@@ -2983,29 +3006,29 @@
         <v>164</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="22" customFormat="1">
+      <c r="A21" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="E21" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" s="23">
         <v>1</v>
       </c>
       <c r="G21" s="6" t="s">
@@ -3030,7 +3053,7 @@
         <v>67</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -3132,7 +3155,7 @@
         <v>23</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -3153,7 +3176,7 @@
         <v>165</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>164</v>
@@ -3176,7 +3199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -3186,7 +3209,7 @@
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.25" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.25" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -3202,12 +3225,12 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G1" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>76</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -3224,19 +3247,19 @@
       <c r="B2" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="13">
         <v>100000</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="J2" s="16">
+        <v>182</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" s="13">
         <v>100000</v>
       </c>
     </row>
@@ -3247,11 +3270,11 @@
       <c r="B3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="13" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3262,13 +3285,13 @@
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>195</v>
+      <c r="C4" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="13" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3279,13 +3302,13 @@
       <c r="B5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>196</v>
+      <c r="C5" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3296,18 +3319,18 @@
       <c r="B6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="3" t="s">
         <v>83</v>
       </c>
       <c r="G6" t="s">
-        <v>185</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>195</v>
+        <v>183</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3317,17 +3340,17 @@
       <c r="B7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>197</v>
+      <c r="C7" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>218</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3337,18 +3360,18 @@
       <c r="B8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>196</v>
+      <c r="H8" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3358,13 +3381,13 @@
       <c r="B9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>198</v>
+      <c r="C9" s="13" t="s">
+        <v>196</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="15" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3375,19 +3398,19 @@
       <c r="B10" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="19"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16" t="s">
-        <v>197</v>
+      <c r="G10" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3397,13 +3420,13 @@
       <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>199</v>
+      <c r="C11" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="13" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3414,20 +3437,20 @@
       <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>206</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>198</v>
+        <v>204</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3437,37 +3460,37 @@
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>199</v>
+      <c r="G14" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3477,19 +3500,19 @@
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>202</v>
+      <c r="C15" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G15" t="s">
-        <v>208</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="J15" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="J15" s="13" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3500,18 +3523,18 @@
       <c r="B16" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C16" s="19"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>200</v>
+      <c r="G16" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3519,20 +3542,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C17" s="19"/>
+        <v>214</v>
+      </c>
+      <c r="C17" s="16"/>
       <c r="D17" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G17" t="s">
-        <v>211</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>201</v>
+        <v>209</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3542,18 +3565,18 @@
       <c r="B18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="19"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>202</v>
+      <c r="G18" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3563,11 +3586,11 @@
       <c r="B19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="19"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I19" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3578,11 +3601,11 @@
       <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>203</v>
+      <c r="C20" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3592,11 +3615,11 @@
       <c r="B21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>204</v>
+      <c r="C21" s="13" t="s">
+        <v>202</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:10">

</xml_diff>